<commit_message>
Populated tables pets and pack_animals.
</commit_message>
<xml_diff>
--- a/OOP/ClassDiagram/data.xlsx
+++ b/OOP/ClassDiagram/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GB_C-SharpDeveloper\01-Итоговая контрольная работа\OOP\ClassDiagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152326E-220D-4252-82CD-692DC2628812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D125E-B4E9-4182-B876-B14C577C8E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{81D80B9E-B475-4C9D-B9A8-1D742F031FF5}"/>
   </bookViews>
@@ -206,8 +206,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -275,16 +284,16 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,332 +611,332 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="1.88671875" customWidth="1"/>
     <col min="8" max="8" width="1.44140625" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="22.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2">
         <v>550</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3">
         <v>610</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4">
         <v>205</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5">
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5">
         <v>730</v>
-      </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6">
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6">
         <v>375</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7">
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7">
         <v>820</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8">
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8">
         <v>1000</v>
-      </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9">
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9">
         <v>790</v>
-      </c>
-      <c r="L9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{2EB17176-D4DE-4561-A054-4EFC001FABF1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{2EB17176-D4DE-4561-A054-4EFC001FABF1}">
       <formula1>$G$2:$G$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{B4611D80-E572-44DA-AABA-9CCF33E31B11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{B4611D80-E572-44DA-AABA-9CCF33E31B11}">
       <formula1>$I$2:$I$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Created table 'animal_age', calculated each animal age.
</commit_message>
<xml_diff>
--- a/OOP/ClassDiagram/data.xlsx
+++ b/OOP/ClassDiagram/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GB_C-SharpDeveloper\01-Итоговая контрольная работа\OOP\ClassDiagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D125E-B4E9-4182-B876-B14C577C8E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0EB7EF-A07A-48F2-A00A-D14655B92B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{81D80B9E-B475-4C9D-B9A8-1D742F031FF5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>weight</t>
   </si>
@@ -200,12 +200,57 @@
   </si>
   <si>
     <t>Черныш</t>
+  </si>
+  <si>
+    <t>волк</t>
+  </si>
+  <si>
+    <t>заяц</t>
+  </si>
+  <si>
+    <t>медведь</t>
+  </si>
+  <si>
+    <t>Малыш</t>
+  </si>
+  <si>
+    <t>Добряк</t>
+  </si>
+  <si>
+    <t>Боня</t>
+  </si>
+  <si>
+    <t>Ракша</t>
+  </si>
+  <si>
+    <t>dif. years</t>
+  </si>
+  <si>
+    <t>dif. months</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>2022-11-02</t>
+  </si>
+  <si>
+    <t>2022-01-06</t>
+  </si>
+  <si>
+    <t>2023-03-30</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F419]yyyy\,\ mmmm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,12 +270,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -282,18 +345,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,336 +707,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6A7F7C-B0DC-4A72-8780-19C4C521ED60}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="1.88671875" customWidth="1"/>
     <col min="8" max="8" width="1.44140625" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="22.21875" customWidth="1"/>
+    <col min="16" max="16" width="1.88671875" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="22" max="22" width="2" customWidth="1"/>
+    <col min="24" max="24" width="1.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.21875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="15" t="s">
         <v>0</v>
       </c>
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="6" t="str">
+        <f>S1</f>
+        <v>birth_date</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="24">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="18">
         <v>550</v>
       </c>
+      <c r="Q2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9">
+        <v>41</v>
+      </c>
+      <c r="V2" s="9"/>
+      <c r="W2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="12">
+        <v>44867</v>
+      </c>
+      <c r="Z2" s="12">
+        <f ca="1">NOW()</f>
+        <v>45662.976429282404</v>
+      </c>
+      <c r="AA2" s="9">
+        <f ca="1">DATEDIF(Y2, Z2, "y")</f>
+        <v>2</v>
+      </c>
+      <c r="AB2" s="9">
+        <f ca="1">DATEDIF(Y2, Z2, "ym")</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="24">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="18">
         <v>610</v>
       </c>
+      <c r="Q3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9">
+        <v>110</v>
+      </c>
+      <c r="V3" s="9"/>
+      <c r="W3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="12">
+        <v>44567</v>
+      </c>
+      <c r="Z3" s="12">
+        <f t="shared" ref="Z3:Z5" ca="1" si="0">NOW()</f>
+        <v>45662.976429282404</v>
+      </c>
+      <c r="AA3" s="9">
+        <f t="shared" ref="AA3:AA5" ca="1" si="1">DATEDIF(Y3, Z3, "y")</f>
+        <v>2</v>
+      </c>
+      <c r="AB3" s="9">
+        <f t="shared" ref="AB3:AB5" ca="1" si="2">DATEDIF(Y3, Z3, "ym")</f>
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="18">
         <v>205</v>
       </c>
+      <c r="Q4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9">
+        <v>70</v>
+      </c>
+      <c r="V4" s="9"/>
+      <c r="W4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="12">
+        <v>45015</v>
+      </c>
+      <c r="Z4" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45662.976429282404</v>
+      </c>
+      <c r="AA4" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB4" s="9">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="24">
         <v>2</v>
       </c>
-      <c r="K5" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="18">
         <v>730</v>
       </c>
+      <c r="Q5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9">
+        <v>3</v>
+      </c>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="12">
+        <v>45267</v>
+      </c>
+      <c r="Z5" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>45662.976429282404</v>
+      </c>
+      <c r="AA5" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB5" s="9">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="24">
         <v>5</v>
       </c>
-      <c r="K6" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="18">
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="24">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="18">
         <v>820</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="24">
         <v>6</v>
       </c>
-      <c r="K8" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="18">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="24">
         <v>2</v>
       </c>
-      <c r="K9" t="s">
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="18">
         <v>790</v>
       </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="R15" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{2EB17176-D4DE-4561-A054-4EFC001FABF1}">
       <formula1>$G$2:$G$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{B4611D80-E572-44DA-AABA-9CCF33E31B11}">
       <formula1>$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{27C4F7F8-B38F-43CF-8A9C-CCBC7CC4D568}">
+      <formula1>$W$2:$W$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>